<commit_message>
Pure adjusted. Renorm Isotherm
</commit_message>
<xml_diff>
--- a/Planilhas de análise/Programação.xlsx
+++ b/Planilhas de análise/Programação.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7530" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7530"/>
   </bookViews>
   <sheets>
     <sheet name="Original" sheetId="1" r:id="rId1"/>
@@ -291,13 +291,13 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -378,31 +378,31 @@
                   <c:v>42620</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>42623</c:v>
+                  <c:v>42628</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>42626</c:v>
+                  <c:v>42631</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>42629</c:v>
+                  <c:v>42634</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>42632</c:v>
+                  <c:v>42637</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>42635</c:v>
+                  <c:v>42640</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>42638</c:v>
+                  <c:v>42648</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>42641</c:v>
+                  <c:v>42654</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>42645</c:v>
+                  <c:v>42657</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>42652</c:v>
+                  <c:v>42663</c:v>
                 </c:pt>
                 <c:pt idx="12">
                   <c:v>42672</c:v>
@@ -664,7 +664,7 @@
 <chartsheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <sheetPr/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="74" workbookViewId="0" zoomToFit="1"/>
+    <sheetView zoomScale="74" workbookViewId="0" zoomToFit="1"/>
   </sheetViews>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
   <drawing r:id="rId1"/>
@@ -1021,8 +1021,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I68"/>
   <sheetViews>
-    <sheetView topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="I6" sqref="I6"/>
+    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
+      <selection activeCell="J6" sqref="J6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1065,10 +1065,10 @@
       <c r="D2" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="F2" s="13" t="s">
+      <c r="F2" s="14" t="s">
         <v>14</v>
       </c>
-      <c r="G2" s="14"/>
+      <c r="G2" s="15"/>
       <c r="H2" s="12" t="s">
         <v>15</v>
       </c>
@@ -1094,7 +1094,7 @@
       <c r="H3" s="9">
         <v>42614</v>
       </c>
-      <c r="I3" s="15">
+      <c r="I3" s="13">
         <v>42614</v>
       </c>
     </row>
@@ -1116,7 +1116,7 @@
       <c r="H4" s="7">
         <v>42617</v>
       </c>
-      <c r="I4" s="15">
+      <c r="I4" s="13">
         <v>42614</v>
       </c>
     </row>
@@ -1138,7 +1138,7 @@
       <c r="H5" s="9">
         <v>42620</v>
       </c>
-      <c r="I5" s="15">
+      <c r="I5" s="13">
         <v>42614</v>
       </c>
     </row>
@@ -1157,10 +1157,10 @@
       <c r="G6" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="H6" s="7">
-        <v>42623</v>
-      </c>
-      <c r="I6" s="15"/>
+      <c r="H6" s="10">
+        <v>42628</v>
+      </c>
+      <c r="I6" s="13"/>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A7" s="9">
@@ -1177,8 +1177,8 @@
       <c r="G7" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="H7" s="10">
-        <v>42626</v>
+      <c r="H7" s="8">
+        <v>42631</v>
       </c>
       <c r="I7" s="3"/>
     </row>
@@ -1198,7 +1198,7 @@
         <v>11</v>
       </c>
       <c r="H8" s="10">
-        <v>42629</v>
+        <v>42634</v>
       </c>
       <c r="I8" s="3"/>
     </row>
@@ -1217,8 +1217,8 @@
       <c r="G9" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="H9" s="10">
-        <v>42632</v>
+      <c r="H9" s="8">
+        <v>42637</v>
       </c>
       <c r="I9" s="3"/>
     </row>
@@ -1238,7 +1238,7 @@
         <v>13</v>
       </c>
       <c r="H10" s="10">
-        <v>42635</v>
+        <v>42640</v>
       </c>
       <c r="I10" s="3"/>
     </row>
@@ -1257,8 +1257,8 @@
       <c r="G11" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="H11" s="8">
-        <v>42638</v>
+      <c r="H11" s="11">
+        <v>42648</v>
       </c>
       <c r="I11" s="3"/>
     </row>
@@ -1277,8 +1277,8 @@
       <c r="G12" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="H12" s="10">
-        <v>42641</v>
+      <c r="H12" s="11">
+        <v>42654</v>
       </c>
       <c r="I12" s="3"/>
     </row>
@@ -1287,7 +1287,7 @@
         <v>42624</v>
       </c>
       <c r="B13" s="3" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C13" s="3"/>
       <c r="D13" s="3"/>
@@ -1297,8 +1297,8 @@
       <c r="G13" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="H13" s="4">
-        <v>42645</v>
+      <c r="H13" s="11">
+        <v>42657</v>
       </c>
       <c r="I13" s="3"/>
     </row>
@@ -1307,7 +1307,7 @@
         <v>42625</v>
       </c>
       <c r="B14" s="3" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C14" s="3"/>
       <c r="D14" s="3"/>
@@ -1317,8 +1317,8 @@
       <c r="G14" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="H14" s="4">
-        <v>42652</v>
+      <c r="H14" s="11">
+        <v>42663</v>
       </c>
       <c r="I14" s="3"/>
     </row>
@@ -1327,7 +1327,7 @@
         <v>42626</v>
       </c>
       <c r="B15" s="3" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C15" s="3"/>
       <c r="D15" s="3"/>
@@ -1347,7 +1347,7 @@
         <v>42627</v>
       </c>
       <c r="B16" s="3" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="C16" s="3"/>
       <c r="D16" s="3"/>
@@ -1367,7 +1367,7 @@
         <v>42628</v>
       </c>
       <c r="B17" s="3" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="C17" s="3"/>
       <c r="D17" s="3"/>
@@ -1387,7 +1387,7 @@
         <v>42629</v>
       </c>
       <c r="B18" s="3" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C18" s="3"/>
       <c r="D18" s="3"/>
@@ -1397,7 +1397,7 @@
         <v>42630</v>
       </c>
       <c r="B19" s="3" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="C19" s="3"/>
       <c r="D19" s="3"/>
@@ -1407,7 +1407,7 @@
         <v>42631</v>
       </c>
       <c r="B20" s="3" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="C20" s="3"/>
       <c r="D20" s="3"/>
@@ -1417,7 +1417,7 @@
         <v>42632</v>
       </c>
       <c r="B21" s="3" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C21" s="3"/>
       <c r="D21" s="3"/>
@@ -1427,7 +1427,7 @@
         <v>42633</v>
       </c>
       <c r="B22" s="3" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="C22" s="3"/>
       <c r="D22" s="3"/>
@@ -1437,7 +1437,7 @@
         <v>42634</v>
       </c>
       <c r="B23" s="3" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="C23" s="3"/>
       <c r="D23" s="3"/>
@@ -1447,7 +1447,7 @@
         <v>42635</v>
       </c>
       <c r="B24" s="3" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C24" s="3"/>
       <c r="D24" s="3"/>
@@ -1457,7 +1457,7 @@
         <v>42636</v>
       </c>
       <c r="B25" s="3" t="s">
-        <v>17</v>
+        <v>12</v>
       </c>
       <c r="C25" s="3"/>
       <c r="D25" s="3"/>
@@ -1467,7 +1467,7 @@
         <v>42637</v>
       </c>
       <c r="B26" s="3" t="s">
-        <v>17</v>
+        <v>12</v>
       </c>
       <c r="C26" s="3"/>
       <c r="D26" s="3"/>
@@ -1477,7 +1477,7 @@
         <v>42638</v>
       </c>
       <c r="B27" s="3" t="s">
-        <v>17</v>
+        <v>13</v>
       </c>
       <c r="C27" s="3"/>
       <c r="D27" s="3"/>
@@ -1487,7 +1487,7 @@
         <v>42639</v>
       </c>
       <c r="B28" s="3" t="s">
-        <v>18</v>
+        <v>13</v>
       </c>
       <c r="C28" s="3"/>
       <c r="D28" s="3"/>
@@ -1497,7 +1497,7 @@
         <v>42640</v>
       </c>
       <c r="B29" s="3" t="s">
-        <v>18</v>
+        <v>13</v>
       </c>
       <c r="C29" s="3"/>
       <c r="D29" s="3"/>
@@ -1507,7 +1507,7 @@
         <v>42641</v>
       </c>
       <c r="B30" s="3" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C30" s="3"/>
       <c r="D30" s="3"/>
@@ -1517,7 +1517,7 @@
         <v>42642</v>
       </c>
       <c r="B31" s="3" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="C31" s="3"/>
       <c r="D31" s="3"/>
@@ -1527,7 +1527,7 @@
         <v>42643</v>
       </c>
       <c r="B32" s="3" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="C32" s="3"/>
       <c r="D32" s="3"/>
@@ -1537,7 +1537,7 @@
         <v>42644</v>
       </c>
       <c r="B33" s="3" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="C33" s="3"/>
       <c r="D33" s="3"/>
@@ -1547,7 +1547,7 @@
         <v>42645</v>
       </c>
       <c r="B34" s="3" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="C34" s="3"/>
       <c r="D34" s="3"/>
@@ -1557,7 +1557,7 @@
         <v>42646</v>
       </c>
       <c r="B35" s="3" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="C35" s="3"/>
       <c r="D35" s="3"/>
@@ -1567,7 +1567,7 @@
         <v>42647</v>
       </c>
       <c r="B36" s="3" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="C36" s="3"/>
       <c r="D36" s="3"/>
@@ -1577,7 +1577,7 @@
         <v>42648</v>
       </c>
       <c r="B37" s="3" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="C37" s="3"/>
       <c r="D37" s="3"/>
@@ -1587,7 +1587,7 @@
         <v>42649</v>
       </c>
       <c r="B38" s="3" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="C38" s="3"/>
       <c r="D38" s="3"/>
@@ -1597,7 +1597,7 @@
         <v>42650</v>
       </c>
       <c r="B39" s="3" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="C39" s="3"/>
       <c r="D39" s="3"/>
@@ -1607,7 +1607,7 @@
         <v>42651</v>
       </c>
       <c r="B40" s="3" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="C40" s="3"/>
       <c r="D40" s="3"/>
@@ -1617,7 +1617,7 @@
         <v>42652</v>
       </c>
       <c r="B41" s="3" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="C41" s="3"/>
       <c r="D41" s="3"/>
@@ -1627,7 +1627,7 @@
         <v>42653</v>
       </c>
       <c r="B42" s="3" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="C42" s="3"/>
       <c r="D42" s="3"/>
@@ -1637,7 +1637,7 @@
         <v>42654</v>
       </c>
       <c r="B43" s="3" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="C43" s="3"/>
       <c r="D43" s="3"/>
@@ -1647,7 +1647,7 @@
         <v>42655</v>
       </c>
       <c r="B44" s="3" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="C44" s="3"/>
       <c r="D44" s="3"/>
@@ -1657,7 +1657,7 @@
         <v>42656</v>
       </c>
       <c r="B45" s="3" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="C45" s="3"/>
       <c r="D45" s="3"/>
@@ -1667,7 +1667,7 @@
         <v>42657</v>
       </c>
       <c r="B46" s="3" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="C46" s="3"/>
       <c r="D46" s="3"/>
@@ -1677,7 +1677,7 @@
         <v>42658</v>
       </c>
       <c r="B47" s="3" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C47" s="3"/>
       <c r="D47" s="3"/>
@@ -1687,7 +1687,7 @@
         <v>42659</v>
       </c>
       <c r="B48" s="3" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C48" s="3"/>
       <c r="D48" s="3"/>
@@ -1697,7 +1697,7 @@
         <v>42660</v>
       </c>
       <c r="B49" s="3" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C49" s="3"/>
       <c r="D49" s="3"/>
@@ -1707,7 +1707,7 @@
         <v>42661</v>
       </c>
       <c r="B50" s="3" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C50" s="3"/>
       <c r="D50" s="3"/>
@@ -1717,7 +1717,7 @@
         <v>42662</v>
       </c>
       <c r="B51" s="3" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C51" s="3"/>
       <c r="D51" s="3"/>
@@ -1727,7 +1727,7 @@
         <v>42663</v>
       </c>
       <c r="B52" s="3" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C52" s="3"/>
       <c r="D52" s="3"/>

</xml_diff>